<commit_message>
Feature Selection / Highlighting CSV
</commit_message>
<xml_diff>
--- a/Resources/Datasets/INDINF_REAL_ESTATE.xlsx
+++ b/Resources/Datasets/INDINF_REAL_ESTATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_30b2\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\FinTechBootCamp\Group Work\PROJECT2FILES\-fintech-project2-machine-learning\Resources\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D5539DA-80CB-C849-A493-8836C50B967A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1064889B-5CAC-4097-933E-E6B8A5EE0A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="184">
   <si>
     <t>TERMS AND CONDITIONS</t>
   </si>
@@ -580,13 +580,37 @@
   </si>
   <si>
     <t>2021Q3</t>
+  </si>
+  <si>
+    <r>
+      <t>The housing affordability index is meant to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF202124"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>measure the share of disposable income that a representative household would put toward housing-related expenses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF202124"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. The measure is a ratio of housing-related costs (mortgage payments and utility fees) to average household disposable income.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -721,8 +745,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -900,6 +946,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1063,8 +1115,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1420,1769 +1476,1779 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:D184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>0.42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>0.46100000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>0.48199999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>0.53400000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>0.626</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>0.54700000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>0.53700000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>0.505</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>0.42</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>0.38100000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>0.38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>0.36699999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>0.35499999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>0.35</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>0.374</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>0.38900000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="2">
         <v>0.318</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>0.317</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>0.32100000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="2">
         <v>0.32100000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="2">
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="2">
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="2">
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="2">
         <v>0.36599999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="2">
         <v>0.374</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="2">
         <v>0.39</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="2">
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="2">
         <v>0.39700000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="2">
         <v>0.41899999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="2">
         <v>0.43</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="2">
         <v>0.46700000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="2">
         <v>0.47199999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>54</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="2">
         <v>0.46200000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="2">
         <v>0.46800000000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="2">
         <v>0.47899999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>57</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="2">
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>58</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="2">
         <v>0.49399999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>59</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="2">
         <v>0.46700000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>60</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="2">
         <v>0.434</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="2">
         <v>0.434</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>62</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="2">
         <v>0.434</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="2">
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="2">
         <v>0.38600000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>65</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="2">
         <v>0.38200000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>66</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="2">
         <v>0.34</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="2">
         <v>0.36899999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="2">
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="3">
         <v>1.5</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="2">
         <v>0.34100000000000003</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="3">
         <v>1.4</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="2">
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="3">
         <v>1.2</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="2">
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="3">
         <v>0.9</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="2">
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>73</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="3">
         <v>0.1</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="2">
         <v>0.379</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>74</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="3">
         <v>-0.2</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="2">
         <v>0.39800000000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>75</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="3">
         <v>-0.2</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="2">
         <v>0.38800000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>76</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="3">
         <v>-0.4</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="2">
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>77</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="3">
         <v>-0.9</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="2">
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>78</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="3">
         <v>-1.3</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="2">
         <v>0.34100000000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>79</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="3">
         <v>-1.9</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="2">
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>80</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="3">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="2">
         <v>0.318</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>81</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="3">
         <v>-2.4</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="2">
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>82</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="3">
         <v>-2.1</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="2">
         <v>0.317</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>83</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="3">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="2">
         <v>0.29299999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="3">
         <v>-0.1</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="2">
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="3">
         <v>0.9</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="2">
         <v>0.30099999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="2">
         <v>0.28799999999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="2">
         <v>0.28499999999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="2">
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>89</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="3">
         <v>1</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="2">
         <v>0.28399999999999997</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="2">
         <v>0.28100000000000003</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>91</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="3">
         <v>0.8</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="2">
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="3">
         <v>0.6</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="2">
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="3">
         <v>0.5</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="2">
         <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>94</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="3">
         <v>0.8</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="2">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="3">
         <v>1.5</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="2">
         <v>0.29899999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>96</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="3">
         <v>1.8</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="2">
         <v>0.308</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>97</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="3">
         <v>2.4</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="2">
         <v>0.308</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="3">
         <v>2.5</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="2">
         <v>0.30099999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>99</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="3">
         <v>2.5</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="2">
         <v>0.29899999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>100</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="3">
         <v>2.6</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="2">
         <v>0.28100000000000003</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>101</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="3">
         <v>2.8</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="2">
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>102</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="3">
         <v>2.9</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="2">
         <v>0.28100000000000003</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>103</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="3">
         <v>2.7</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="2">
         <v>0.26500000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>104</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="3">
         <v>3.2</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="2">
         <v>0.26300000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="3">
         <v>4</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="2">
         <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>106</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="3">
         <v>4.2</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="2">
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>107</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="2">
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>108</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="2">
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>109</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="2">
         <v>0.28100000000000003</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>110</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="3">
         <v>4.8</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="2">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>111</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="3">
         <v>5</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="2">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>112</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="2">
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>113</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="3">
         <v>5.8</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="2">
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>114</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="3">
         <v>5.9</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="2">
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>115</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="3">
         <v>5.3</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="2">
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C118">
+      <c r="C118" s="2">
         <v>0.29699999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>117</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="3">
         <v>4.7</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="2">
         <v>0.29699999999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>118</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="3">
         <v>4.7</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="2">
         <v>0.29899999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>119</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="3">
         <v>5.6</v>
       </c>
-      <c r="C121">
+      <c r="C121" s="2">
         <v>0.315</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>120</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="3">
         <v>7.1</v>
       </c>
-      <c r="C122">
+      <c r="C122" s="2">
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>121</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="3">
         <v>9.1</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="2">
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>122</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="3">
         <v>11.6</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="2">
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>123</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="3">
         <v>11.2</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="2">
         <v>0.34100000000000003</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>124</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="3">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="2">
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>125</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="3">
         <v>8.4</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="2">
         <v>0.36</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>126</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="3">
         <v>6.8</v>
       </c>
-      <c r="C128">
+      <c r="C128" s="2">
         <v>0.38100000000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>127</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="3">
         <v>6.1</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="2">
         <v>0.38900000000000001</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>128</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="3">
         <v>6.3</v>
       </c>
-      <c r="C130">
+      <c r="C130" s="2">
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>129</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="3">
         <v>4.3</v>
       </c>
-      <c r="C131">
+      <c r="C131" s="2">
         <v>0.36199999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>130</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C132">
+      <c r="C132" s="2">
         <v>0.34699999999999998</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>131</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="3">
         <v>0.9</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="2">
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>132</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="3">
         <v>-1.6</v>
       </c>
-      <c r="C134">
+      <c r="C134" s="2">
         <v>0.307</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>133</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="3">
         <v>-3.1</v>
       </c>
-      <c r="C135">
+      <c r="C135" s="2">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>134</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="3">
         <v>-3</v>
       </c>
-      <c r="C136">
+      <c r="C136" s="2">
         <v>0.30299999999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>135</v>
       </c>
-      <c r="B137">
+      <c r="B137" s="3">
         <v>-1.5</v>
       </c>
-      <c r="C137">
+      <c r="C137" s="2">
         <v>0.309</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>136</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="3">
         <v>0.8</v>
       </c>
-      <c r="C138">
+      <c r="C138" s="2">
         <v>0.30399999999999999</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>137</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="3">
         <v>2.9</v>
       </c>
-      <c r="C139">
+      <c r="C139" s="2">
         <v>0.318</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>138</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="3">
         <v>2.8</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="2">
         <v>0.307</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>139</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C141">
+      <c r="C141" s="2">
         <v>0.30199999999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>140</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="3">
         <v>1.9</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="2">
         <v>0.314</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>141</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="3">
         <v>1.9</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="2">
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>142</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C144">
+      <c r="C144" s="2">
         <v>0.318</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>143</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="3">
         <v>2.5</v>
       </c>
-      <c r="C145">
+      <c r="C145" s="2">
         <v>0.315</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>144</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="3">
         <v>2.4</v>
       </c>
-      <c r="C146">
+      <c r="C146" s="2">
         <v>0.313</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>145</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="3">
         <v>2.4</v>
       </c>
-      <c r="C147">
+      <c r="C147" s="2">
         <v>0.312</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>146</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="3">
         <v>2.4</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="2">
         <v>0.30599999999999999</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>147</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C149">
+      <c r="C149" s="2">
         <v>0.30399999999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>148</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="3">
         <v>2.1</v>
       </c>
-      <c r="C150">
+      <c r="C150" s="2">
         <v>0.29899999999999999</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>149</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="3">
         <v>1.8</v>
       </c>
-      <c r="C151">
+      <c r="C151" s="2">
         <v>0.30299999999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>150</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="3">
         <v>1.7</v>
       </c>
-      <c r="C152">
+      <c r="C152" s="2">
         <v>0.313</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>151</v>
       </c>
-      <c r="B153">
+      <c r="B153" s="3">
         <v>1.4</v>
       </c>
-      <c r="C153">
+      <c r="C153" s="2">
         <v>0.32100000000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>152</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="3">
         <v>1.5</v>
       </c>
-      <c r="C154">
+      <c r="C154" s="2">
         <v>0.32100000000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>153</v>
       </c>
-      <c r="B155">
+      <c r="B155" s="3">
         <v>1.5</v>
       </c>
-      <c r="C155">
+      <c r="C155" s="2">
         <v>0.318</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>154</v>
       </c>
-      <c r="B156">
+      <c r="B156" s="3">
         <v>1.5</v>
       </c>
-      <c r="C156">
+      <c r="C156" s="2">
         <v>0.313</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>155</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="3">
         <v>1.7</v>
       </c>
-      <c r="C157">
+      <c r="C157" s="2">
         <v>0.318</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>156</v>
       </c>
-      <c r="B158">
+      <c r="B158" s="3">
         <v>1.3</v>
       </c>
-      <c r="C158">
+      <c r="C158" s="2">
         <v>0.312</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>157</v>
       </c>
-      <c r="B159">
+      <c r="B159" s="3">
         <v>1.2</v>
       </c>
-      <c r="C159">
+      <c r="C159" s="2">
         <v>0.31</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>158</v>
       </c>
-      <c r="B160">
+      <c r="B160" s="3">
         <v>1.4</v>
       </c>
-      <c r="C160">
+      <c r="C160" s="2">
         <v>0.314</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>159</v>
       </c>
-      <c r="B161">
+      <c r="B161" s="3">
         <v>1.5</v>
       </c>
-      <c r="C161">
+      <c r="C161" s="2">
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>160</v>
       </c>
-      <c r="B162">
+      <c r="B162" s="3">
         <v>1.8</v>
       </c>
-      <c r="C162">
+      <c r="C162" s="2">
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>161</v>
       </c>
-      <c r="B163">
+      <c r="B163" s="3">
         <v>2.5</v>
       </c>
-      <c r="C163">
+      <c r="C163" s="2">
         <v>0.35</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>162</v>
       </c>
-      <c r="B164">
+      <c r="B164" s="3">
         <v>2.8</v>
       </c>
-      <c r="C164">
+      <c r="C164" s="2">
         <v>0.34699999999999998</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>163</v>
       </c>
-      <c r="B165">
+      <c r="B165" s="3">
         <v>3.1</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="2">
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>164</v>
       </c>
-      <c r="B166">
+      <c r="B166" s="3">
         <v>3.2</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="2">
         <v>0.35</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>165</v>
       </c>
-      <c r="B167">
+      <c r="B167" s="3">
         <v>3.8</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="2">
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>166</v>
       </c>
-      <c r="B168">
+      <c r="B168" s="3">
         <v>3.8</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="2">
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>167</v>
       </c>
-      <c r="B169">
+      <c r="B169" s="3">
         <v>3.4</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="2">
         <v>0.34699999999999998</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>168</v>
       </c>
-      <c r="B170">
+      <c r="B170" s="3">
         <v>2.7</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="2">
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>169</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C171">
+      <c r="C171" s="2">
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>170</v>
       </c>
-      <c r="B172">
+      <c r="B172" s="3">
         <v>0.4</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="2">
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>171</v>
       </c>
-      <c r="B173">
+      <c r="B173" s="3">
         <v>0</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="2">
         <v>0.35799999999999998</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>172</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="3">
         <v>0</v>
       </c>
-      <c r="C174">
+      <c r="C174" s="2">
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>173</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="3">
         <v>0</v>
       </c>
-      <c r="C175">
+      <c r="C175" s="2">
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>174</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="3">
         <v>-0.3</v>
       </c>
-      <c r="C176">
+      <c r="C176" s="2">
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>175</v>
       </c>
-      <c r="B177">
+      <c r="B177" s="3">
         <v>0</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="2">
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>176</v>
       </c>
-      <c r="B178">
+      <c r="B178" s="3">
         <v>0.5</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="2">
         <v>0.35399999999999998</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>177</v>
       </c>
-      <c r="B179">
+      <c r="B179" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>178</v>
       </c>
-      <c r="B180">
+      <c r="B180" s="3">
         <v>2.4</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="2">
         <v>0.315</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>179</v>
       </c>
-      <c r="B181">
+      <c r="B181" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="2">
         <v>0.33700000000000002</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>180</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="3">
         <v>6.8</v>
       </c>
-      <c r="C182">
+      <c r="C182" s="2">
         <v>0.34699999999999998</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>181</v>
       </c>
-      <c r="B183">
+      <c r="B183" s="3">
         <v>11</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="2">
         <v>0.36299999999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>182</v>
       </c>
-      <c r="B184">
+      <c r="B184" s="3">
         <v>11.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>